<commit_message>
Show unconnected pins on connectors.
</commit_message>
<xml_diff>
--- a/Altoid MIDI Box Wiring.xlsx
+++ b/Altoid MIDI Box Wiring.xlsx
@@ -128,7 +128,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -170,6 +170,11 @@
     <font>
       <sz val="8"/>
       <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="21"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -246,7 +251,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="85">
+  <borders count="108">
     <border>
       <left/>
       <right/>
@@ -925,9 +930,69 @@
     </border>
     <border>
       <left style="thick">
-        <color indexed="8"/>
+        <color indexed="14"/>
+      </left>
+      <right style="medium">
+        <color indexed="14"/>
+      </right>
+      <top style="medium">
+        <color indexed="12"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="14"/>
       </left>
       <right style="thick">
+        <color indexed="12"/>
+      </right>
+      <top style="medium">
+        <color indexed="12"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="12"/>
+      </left>
+      <right style="dotted">
+        <color indexed="14"/>
+      </right>
+      <top style="medium">
+        <color indexed="12"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="14"/>
+      </left>
+      <right style="thick">
+        <color indexed="14"/>
+      </right>
+      <top style="medium">
+        <color indexed="12"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="20"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="8"/>
+      </left>
+      <right style="thick">
         <color indexed="8"/>
       </right>
       <top style="thin">
@@ -939,13 +1004,178 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="12"/>
+      </left>
+      <right style="medium">
+        <color indexed="20"/>
+      </right>
+      <top style="medium">
+        <color indexed="12"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="20"/>
+      </left>
+      <right style="medium">
+        <color indexed="20"/>
+      </right>
+      <top style="medium">
+        <color indexed="20"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="20"/>
+      </left>
+      <right style="thick">
+        <color indexed="12"/>
+      </right>
+      <top style="medium">
+        <color indexed="12"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="14"/>
+      </left>
+      <right style="thick">
+        <color indexed="14"/>
+      </right>
+      <top style="medium">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="8"/>
+      </left>
+      <right style="thick">
+        <color indexed="8"/>
+      </right>
+      <top style="thick">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="14"/>
+      </left>
+      <right style="thick">
+        <color indexed="14"/>
+      </right>
+      <top style="medium">
+        <color indexed="22"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thick">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thick">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="medium">
+        <color indexed="12"/>
+      </right>
+      <top style="thick">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thick">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="14"/>
+      </left>
       <right style="thick">
-        <color indexed="8"/>
+        <color indexed="14"/>
       </right>
       <top style="thick">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thick">
+        <color indexed="8"/>
+      </right>
+      <top style="thick">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
@@ -957,6 +1187,21 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="medium">
+        <color indexed="22"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right style="thick">
         <color indexed="12"/>
       </right>
@@ -969,17 +1214,47 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thick">
+        <color indexed="22"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thick">
-        <color indexed="12"/>
+        <color indexed="8"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thick">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="medium">
         <color indexed="12"/>
       </top>
       <bottom style="thick">
-        <color indexed="12"/>
+        <color indexed="23"/>
       </bottom>
       <diagonal/>
     </border>
@@ -990,32 +1265,107 @@
       <right style="thin">
         <color indexed="10"/>
       </right>
+      <top style="medium">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="14"/>
+      </left>
+      <right style="thick">
+        <color indexed="14"/>
+      </right>
       <top style="thick">
-        <color indexed="12"/>
+        <color indexed="23"/>
       </top>
       <bottom style="thick">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="medium">
-        <color indexed="12"/>
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="14"/>
+      </left>
+      <right style="thick">
+        <color indexed="14"/>
       </right>
       <top style="thick">
-        <color indexed="12"/>
+        <color indexed="22"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="14"/>
+      </left>
+      <right style="thick">
+        <color indexed="12"/>
+      </right>
+      <top style="medium">
+        <color indexed="12"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="14"/>
+      </left>
+      <right style="thick">
+        <color indexed="22"/>
+      </right>
+      <top style="medium">
+        <color indexed="22"/>
       </top>
       <bottom style="thick">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="12"/>
+        <color indexed="24"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="22"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
@@ -1030,16 +1380,16 @@
     </border>
     <border>
       <left style="thick">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
+        <color indexed="14"/>
+      </left>
+      <right style="thick">
+        <color indexed="12"/>
       </right>
       <top style="thick">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="24"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1446,7 +1796,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="192">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1666,10 +2016,10 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="10" borderId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="49" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="10" borderId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1696,10 +2046,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="11" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="50" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="11" borderId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1729,52 +2079,76 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="48" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="52" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" borderId="53" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" borderId="54" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="55" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="57" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="58" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="49" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="50" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="51" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="52" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="53" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="54" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="55" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="59" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="60" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="61" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="62" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="63" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="43" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="64" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="65" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="66" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="67" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="68" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1783,10 +2157,34 @@
     <xf numFmtId="0" fontId="5" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" borderId="69" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="70" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="71" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="57" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="72" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="73" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="37" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="74" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1795,7 +2193,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="77" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1804,7 +2205,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1816,112 +2217,112 @@
     <xf numFmtId="49" fontId="4" fillId="7" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="49" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" borderId="64" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="38" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="56" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="57" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="58" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="79" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="80" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="81" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="44" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="60" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="61" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="62" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="63" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="64" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="65" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="66" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="67" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="68" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="69" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="70" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="71" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="72" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="73" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="74" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="75" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="75" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="75" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="82" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="83" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="84" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="85" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="86" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="87" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="88" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="89" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="90" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="91" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="92" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="93" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="94" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="95" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="96" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="97" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="98" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="98" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="98" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="77" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="99" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="100" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="11" borderId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="78" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="99" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="99" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="99" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="99" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="99" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="99" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="11" borderId="99" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="101" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1930,46 +2331,46 @@
     <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="79" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="80" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="81" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="74" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="82" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="83" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="83" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="83" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="83" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="83" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="83" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="84" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="78" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="83" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" borderId="102" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="103" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="104" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="97" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" borderId="105" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="106" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="106" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="106" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="106" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="106" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="106" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="107" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="101" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="106" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -2000,6 +2401,11 @@
       <rgbColor rgb="ff990000"/>
       <rgbColor rgb="ff00ff00"/>
       <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ff04147f"/>
+      <rgbColor rgb="ff5d7f69"/>
+      <rgbColor rgb="ffcc5700"/>
+      <rgbColor rgb="ffff8d00"/>
+      <rgbColor rgb="ffff9140"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -2018,7 +2424,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>234950</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>194530</xdr:rowOff>
+      <xdr:rowOff>181830</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2028,7 +2434,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2051050" y="205395"/>
-          <a:ext cx="1676401" cy="1417886"/>
+          <a:ext cx="1676400" cy="1417886"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2072,7 +2478,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>115743</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>21175</xdr:rowOff>
+      <xdr:rowOff>8475</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3275,7 +3681,7 @@
       </c>
       <c r="S2" s="29"/>
     </row>
-    <row r="3" ht="15.65" customHeight="1">
+    <row r="3" ht="16.15" customHeight="1">
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="32"/>
@@ -3306,7 +3712,7 @@
       <c r="R3" s="45"/>
       <c r="S3" s="46"/>
     </row>
-    <row r="4" ht="15.65" customHeight="1">
+    <row r="4" ht="16.15" customHeight="1">
       <c r="A4" t="s" s="47">
         <v>6</v>
       </c>
@@ -3511,73 +3917,77 @@
       </c>
       <c r="S8" s="94"/>
     </row>
-    <row r="9" ht="15.65" customHeight="1">
+    <row r="9" ht="16.15" customHeight="1">
       <c r="A9" s="103"/>
       <c r="B9" t="s" s="62">
         <v>7</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="104"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="107"/>
+      <c r="C9" s="104"/>
+      <c r="D9" t="s" s="105">
+        <v>2</v>
+      </c>
+      <c r="E9" s="106"/>
+      <c r="F9" s="107"/>
+      <c r="G9" s="108"/>
+      <c r="H9" s="109"/>
       <c r="I9" s="32"/>
       <c r="J9" s="33"/>
       <c r="K9" s="34"/>
-      <c r="L9" s="108"/>
-      <c r="M9" s="106"/>
-      <c r="N9" s="107"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="34"/>
+      <c r="L9" s="110"/>
+      <c r="M9" s="108"/>
+      <c r="N9" s="109"/>
+      <c r="O9" s="104"/>
+      <c r="P9" t="s" s="111">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="112"/>
       <c r="R9" t="s" s="71">
         <v>3</v>
       </c>
-      <c r="S9" s="109"/>
+      <c r="S9" s="103"/>
     </row>
-    <row r="10" ht="15.65" customHeight="1">
-      <c r="A10" s="110"/>
+    <row r="10" ht="16.15" customHeight="1">
+      <c r="A10" s="113"/>
       <c r="B10" t="s" s="62">
         <v>9</v>
       </c>
       <c r="C10" s="32"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="106"/>
-      <c r="H10" s="107"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="115"/>
+      <c r="F10" s="107"/>
+      <c r="G10" s="108"/>
+      <c r="H10" s="109"/>
       <c r="I10" s="32"/>
       <c r="J10" s="33"/>
       <c r="K10" s="34"/>
-      <c r="L10" s="108"/>
-      <c r="M10" s="106"/>
-      <c r="N10" s="107"/>
+      <c r="L10" s="110"/>
+      <c r="M10" s="108"/>
+      <c r="N10" s="109"/>
       <c r="O10" s="32"/>
-      <c r="P10" s="33"/>
+      <c r="P10" s="116"/>
       <c r="Q10" s="34"/>
       <c r="R10" t="s" s="71">
         <v>4</v>
       </c>
-      <c r="S10" s="29"/>
+      <c r="S10" s="117"/>
     </row>
     <row r="11" ht="15.65" customHeight="1">
-      <c r="A11" s="110"/>
+      <c r="A11" s="118"/>
       <c r="B11" t="s" s="62">
         <v>3</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="33"/>
-      <c r="E11" s="104"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="107"/>
+      <c r="E11" s="115"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="108"/>
+      <c r="H11" s="109"/>
       <c r="I11" s="32"/>
       <c r="J11" s="33"/>
       <c r="K11" s="34"/>
-      <c r="L11" s="108"/>
-      <c r="M11" s="106"/>
-      <c r="N11" s="107"/>
+      <c r="L11" s="110"/>
+      <c r="M11" s="108"/>
+      <c r="N11" s="109"/>
       <c r="O11" s="32"/>
       <c r="P11" s="33"/>
       <c r="Q11" s="34"/>
@@ -3587,114 +3997,118 @@
       <c r="S11" s="29"/>
     </row>
     <row r="12" ht="15.65" customHeight="1">
-      <c r="A12" s="110"/>
+      <c r="A12" s="119"/>
       <c r="B12" t="s" s="62">
         <v>12</v>
       </c>
       <c r="C12" s="32"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="104"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="106"/>
-      <c r="H12" s="107"/>
+      <c r="D12" s="120"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="108"/>
+      <c r="H12" s="109"/>
       <c r="I12" s="32"/>
       <c r="J12" s="33"/>
       <c r="K12" s="34"/>
-      <c r="L12" s="108"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="107"/>
+      <c r="L12" s="110"/>
+      <c r="M12" s="108"/>
+      <c r="N12" s="109"/>
       <c r="O12" s="32"/>
-      <c r="P12" s="33"/>
+      <c r="P12" s="121"/>
       <c r="Q12" s="34"/>
       <c r="R12" t="s" s="71">
         <v>8</v>
       </c>
-      <c r="S12" s="29"/>
+      <c r="S12" s="122"/>
     </row>
     <row r="13" ht="15.65" customHeight="1">
-      <c r="A13" s="111"/>
+      <c r="A13" t="s" s="123">
+        <v>18</v>
+      </c>
       <c r="B13" t="s" s="62">
         <v>7</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="106"/>
-      <c r="H13" s="107"/>
+      <c r="C13" s="104"/>
+      <c r="D13" t="s" s="124">
+        <v>2</v>
+      </c>
+      <c r="E13" s="106"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="108"/>
+      <c r="H13" s="109"/>
       <c r="I13" s="32"/>
       <c r="J13" s="33"/>
       <c r="K13" s="34"/>
-      <c r="L13" s="108"/>
-      <c r="M13" s="106"/>
-      <c r="N13" s="107"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="34"/>
+      <c r="L13" s="110"/>
+      <c r="M13" s="108"/>
+      <c r="N13" s="109"/>
+      <c r="O13" s="104"/>
+      <c r="P13" t="s" s="111">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="112"/>
       <c r="R13" t="s" s="71">
         <v>3</v>
       </c>
-      <c r="S13" s="46"/>
+      <c r="S13" t="s" s="125">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" ht="15.65" customHeight="1">
-      <c r="A14" t="s" s="47">
-        <v>18</v>
-      </c>
+      <c r="A14" s="126"/>
       <c r="B14" t="s" s="62">
         <v>7</v>
       </c>
-      <c r="C14" s="112"/>
-      <c r="D14" t="s" s="101">
+      <c r="C14" s="127"/>
+      <c r="D14" t="s" s="128">
         <v>17</v>
       </c>
-      <c r="E14" s="113">
+      <c r="E14" s="129">
         <v>1</v>
       </c>
-      <c r="F14" s="105"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="107"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="108"/>
+      <c r="H14" s="109"/>
       <c r="I14" s="32"/>
       <c r="J14" s="33"/>
       <c r="K14" s="34"/>
-      <c r="L14" s="108"/>
-      <c r="M14" s="106"/>
-      <c r="N14" s="107"/>
-      <c r="O14" s="114">
+      <c r="L14" s="110"/>
+      <c r="M14" s="108"/>
+      <c r="N14" s="109"/>
+      <c r="O14" s="130">
         <v>10</v>
       </c>
-      <c r="P14" t="s" s="101">
+      <c r="P14" t="s" s="128">
         <v>17</v>
       </c>
       <c r="Q14" s="102"/>
       <c r="R14" t="s" s="71">
         <v>3</v>
       </c>
-      <c r="S14" t="s" s="47">
-        <v>19</v>
-      </c>
+      <c r="S14" s="126"/>
     </row>
     <row r="15" ht="15.65" customHeight="1">
       <c r="A15" s="61"/>
       <c r="B15" t="s" s="62">
         <v>7</v>
       </c>
-      <c r="C15" s="115"/>
+      <c r="C15" s="131"/>
       <c r="D15" t="s" s="92">
         <v>16</v>
       </c>
-      <c r="E15" s="116">
+      <c r="E15" s="132">
         <v>2</v>
       </c>
-      <c r="F15" s="105"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="107"/>
+      <c r="F15" s="133"/>
+      <c r="G15" s="108"/>
+      <c r="H15" s="109"/>
       <c r="I15" s="32"/>
       <c r="J15" s="33"/>
       <c r="K15" s="34"/>
-      <c r="L15" s="108"/>
-      <c r="M15" s="106"/>
-      <c r="N15" s="107"/>
-      <c r="O15" s="117">
+      <c r="L15" s="110"/>
+      <c r="M15" s="108"/>
+      <c r="N15" s="109"/>
+      <c r="O15" s="134">
         <v>0</v>
       </c>
       <c r="P15" t="s" s="92">
@@ -3711,23 +4125,23 @@
       <c r="B16" t="s" s="62">
         <v>7</v>
       </c>
-      <c r="C16" s="118"/>
+      <c r="C16" s="135"/>
       <c r="D16" t="s" s="81">
         <v>14</v>
       </c>
-      <c r="E16" s="119">
+      <c r="E16" s="136">
         <v>3</v>
       </c>
-      <c r="F16" s="105"/>
-      <c r="G16" s="106"/>
-      <c r="H16" s="107"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="108"/>
+      <c r="H16" s="109"/>
       <c r="I16" s="32"/>
       <c r="J16" s="33"/>
       <c r="K16" s="34"/>
-      <c r="L16" s="108"/>
-      <c r="M16" s="106"/>
-      <c r="N16" s="107"/>
-      <c r="O16" s="120">
+      <c r="L16" s="110"/>
+      <c r="M16" s="108"/>
+      <c r="N16" s="109"/>
+      <c r="O16" s="137">
         <v>6</v>
       </c>
       <c r="P16" t="s" s="81">
@@ -3751,15 +4165,15 @@
         <v>7</v>
       </c>
       <c r="E17" s="65"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="107"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="108"/>
+      <c r="H17" s="109"/>
       <c r="I17" s="32"/>
       <c r="J17" s="33"/>
       <c r="K17" s="34"/>
-      <c r="L17" s="108"/>
-      <c r="M17" s="106"/>
-      <c r="N17" s="107"/>
+      <c r="L17" s="110"/>
+      <c r="M17" s="108"/>
+      <c r="N17" s="109"/>
       <c r="O17" t="s" s="63">
         <v>3</v>
       </c>
@@ -3774,7 +4188,7 @@
     </row>
     <row r="18" ht="15.65" customHeight="1">
       <c r="A18" s="94"/>
-      <c r="B18" t="s" s="121">
+      <c r="B18" t="s" s="138">
         <v>7</v>
       </c>
       <c r="C18" s="49"/>
@@ -3784,15 +4198,15 @@
       <c r="E18" t="s" s="51">
         <v>17</v>
       </c>
-      <c r="F18" s="105"/>
-      <c r="G18" s="106"/>
-      <c r="H18" s="107"/>
+      <c r="F18" s="107"/>
+      <c r="G18" s="108"/>
+      <c r="H18" s="109"/>
       <c r="I18" s="32"/>
       <c r="J18" s="33"/>
       <c r="K18" s="34"/>
-      <c r="L18" s="108"/>
-      <c r="M18" s="106"/>
-      <c r="N18" s="107"/>
+      <c r="L18" s="110"/>
+      <c r="M18" s="108"/>
+      <c r="N18" s="109"/>
       <c r="O18" s="49"/>
       <c r="P18" t="s" s="50">
         <v>3</v>
@@ -3800,498 +4214,498 @@
       <c r="Q18" t="s" s="59">
         <v>10</v>
       </c>
-      <c r="R18" t="s" s="122">
+      <c r="R18" t="s" s="139">
         <v>10</v>
       </c>
       <c r="S18" s="94"/>
     </row>
     <row r="19" ht="15.65" customHeight="1">
-      <c r="A19" s="123"/>
-      <c r="B19" s="124"/>
+      <c r="A19" s="140"/>
+      <c r="B19" s="141"/>
       <c r="C19" s="32"/>
-      <c r="D19" s="125"/>
-      <c r="E19" s="126"/>
-      <c r="F19" s="105"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="107"/>
+      <c r="D19" s="142"/>
+      <c r="E19" s="143"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="109"/>
       <c r="I19" s="32"/>
       <c r="J19" s="33"/>
       <c r="K19" s="34"/>
-      <c r="L19" s="108"/>
-      <c r="M19" s="106"/>
-      <c r="N19" s="107"/>
-      <c r="O19" s="127"/>
-      <c r="P19" s="125"/>
+      <c r="L19" s="110"/>
+      <c r="M19" s="108"/>
+      <c r="N19" s="109"/>
+      <c r="O19" s="144"/>
+      <c r="P19" s="142"/>
       <c r="Q19" s="34"/>
-      <c r="R19" s="128"/>
-      <c r="S19" s="109"/>
+      <c r="R19" s="145"/>
+      <c r="S19" s="117"/>
     </row>
     <row r="20" ht="15.65" customHeight="1">
       <c r="A20" s="11"/>
-      <c r="B20" t="s" s="129">
+      <c r="B20" t="s" s="146">
         <v>1</v>
       </c>
-      <c r="C20" s="130"/>
-      <c r="D20" s="131"/>
-      <c r="E20" s="132"/>
-      <c r="F20" s="133"/>
-      <c r="G20" s="134"/>
-      <c r="H20" s="135"/>
-      <c r="I20" s="136"/>
-      <c r="J20" s="137"/>
-      <c r="K20" s="138"/>
-      <c r="L20" s="139"/>
-      <c r="M20" s="134"/>
-      <c r="N20" s="140"/>
-      <c r="O20" s="131"/>
-      <c r="P20" s="141"/>
-      <c r="Q20" s="142"/>
-      <c r="R20" t="s" s="143">
+      <c r="C20" s="147"/>
+      <c r="D20" s="148"/>
+      <c r="E20" s="149"/>
+      <c r="F20" s="150"/>
+      <c r="G20" s="151"/>
+      <c r="H20" s="152"/>
+      <c r="I20" s="153"/>
+      <c r="J20" s="154"/>
+      <c r="K20" s="155"/>
+      <c r="L20" s="156"/>
+      <c r="M20" s="151"/>
+      <c r="N20" s="157"/>
+      <c r="O20" s="148"/>
+      <c r="P20" s="158"/>
+      <c r="Q20" s="159"/>
+      <c r="R20" t="s" s="160">
         <v>1</v>
       </c>
       <c r="S20" s="29"/>
     </row>
     <row r="21" ht="14.65" customHeight="1">
-      <c r="A21" s="144"/>
-      <c r="B21" s="145"/>
-      <c r="C21" s="145"/>
-      <c r="D21" s="145"/>
-      <c r="E21" s="145"/>
-      <c r="F21" t="s" s="146">
+      <c r="A21" s="161"/>
+      <c r="B21" s="162"/>
+      <c r="C21" s="162"/>
+      <c r="D21" s="162"/>
+      <c r="E21" s="162"/>
+      <c r="F21" t="s" s="163">
         <v>20</v>
       </c>
-      <c r="G21" s="147"/>
-      <c r="H21" s="147"/>
-      <c r="I21" s="147"/>
-      <c r="J21" s="147"/>
-      <c r="K21" s="147"/>
-      <c r="L21" s="147"/>
-      <c r="M21" s="147"/>
-      <c r="N21" s="147"/>
-      <c r="O21" s="145"/>
-      <c r="P21" s="145"/>
-      <c r="Q21" s="145"/>
-      <c r="R21" s="145"/>
+      <c r="G21" s="164"/>
+      <c r="H21" s="164"/>
+      <c r="I21" s="164"/>
+      <c r="J21" s="164"/>
+      <c r="K21" s="164"/>
+      <c r="L21" s="164"/>
+      <c r="M21" s="164"/>
+      <c r="N21" s="164"/>
+      <c r="O21" s="162"/>
+      <c r="P21" s="162"/>
+      <c r="Q21" s="162"/>
+      <c r="R21" s="162"/>
       <c r="S21" s="10"/>
     </row>
     <row r="22" ht="13.65" customHeight="1">
-      <c r="A22" t="s" s="148">
+      <c r="A22" t="s" s="165">
         <v>21</v>
       </c>
-      <c r="B22" s="149"/>
-      <c r="C22" s="150"/>
-      <c r="D22" s="150"/>
-      <c r="E22" s="150"/>
-      <c r="F22" s="150"/>
-      <c r="G22" s="150"/>
-      <c r="H22" s="150"/>
-      <c r="I22" s="150"/>
-      <c r="J22" s="150"/>
-      <c r="K22" s="150"/>
-      <c r="L22" s="150"/>
-      <c r="M22" s="150"/>
-      <c r="N22" s="150"/>
-      <c r="O22" s="150"/>
-      <c r="P22" s="150"/>
-      <c r="Q22" s="150"/>
-      <c r="R22" s="150"/>
+      <c r="B22" s="166"/>
+      <c r="C22" s="167"/>
+      <c r="D22" s="167"/>
+      <c r="E22" s="167"/>
+      <c r="F22" s="167"/>
+      <c r="G22" s="167"/>
+      <c r="H22" s="167"/>
+      <c r="I22" s="167"/>
+      <c r="J22" s="167"/>
+      <c r="K22" s="167"/>
+      <c r="L22" s="167"/>
+      <c r="M22" s="167"/>
+      <c r="N22" s="167"/>
+      <c r="O22" s="167"/>
+      <c r="P22" s="167"/>
+      <c r="Q22" s="167"/>
+      <c r="R22" s="167"/>
       <c r="S22" s="10"/>
     </row>
     <row r="23" ht="13.65" customHeight="1">
-      <c r="A23" t="s" s="151">
+      <c r="A23" t="s" s="168">
         <v>22</v>
       </c>
-      <c r="B23" s="149"/>
-      <c r="C23" s="150"/>
-      <c r="D23" s="150"/>
-      <c r="E23" s="150"/>
-      <c r="F23" s="150"/>
-      <c r="G23" s="150"/>
-      <c r="H23" s="150"/>
-      <c r="I23" s="150"/>
-      <c r="J23" s="150"/>
-      <c r="K23" s="150"/>
-      <c r="L23" s="150"/>
-      <c r="M23" s="150"/>
-      <c r="N23" s="150"/>
-      <c r="O23" s="150"/>
-      <c r="P23" s="150"/>
-      <c r="Q23" s="150"/>
-      <c r="R23" s="150"/>
+      <c r="B23" s="166"/>
+      <c r="C23" s="167"/>
+      <c r="D23" s="167"/>
+      <c r="E23" s="167"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="167"/>
+      <c r="H23" s="167"/>
+      <c r="I23" s="167"/>
+      <c r="J23" s="167"/>
+      <c r="K23" s="167"/>
+      <c r="L23" s="167"/>
+      <c r="M23" s="167"/>
+      <c r="N23" s="167"/>
+      <c r="O23" s="167"/>
+      <c r="P23" s="167"/>
+      <c r="Q23" s="167"/>
+      <c r="R23" s="167"/>
       <c r="S23" s="10"/>
     </row>
     <row r="24" ht="13.65" customHeight="1">
-      <c r="A24" t="s" s="152">
+      <c r="A24" t="s" s="169">
         <v>23</v>
       </c>
-      <c r="B24" s="149"/>
-      <c r="C24" s="150"/>
-      <c r="D24" s="150"/>
-      <c r="E24" s="150"/>
-      <c r="F24" s="150"/>
-      <c r="G24" s="150"/>
-      <c r="H24" s="150"/>
-      <c r="I24" s="150"/>
-      <c r="J24" s="150"/>
-      <c r="K24" s="150"/>
-      <c r="L24" s="150"/>
-      <c r="M24" s="150"/>
-      <c r="N24" s="150"/>
-      <c r="O24" s="150"/>
-      <c r="P24" s="150"/>
-      <c r="Q24" s="150"/>
-      <c r="R24" s="150"/>
+      <c r="B24" s="166"/>
+      <c r="C24" s="167"/>
+      <c r="D24" s="167"/>
+      <c r="E24" s="167"/>
+      <c r="F24" s="167"/>
+      <c r="G24" s="167"/>
+      <c r="H24" s="167"/>
+      <c r="I24" s="167"/>
+      <c r="J24" s="167"/>
+      <c r="K24" s="167"/>
+      <c r="L24" s="167"/>
+      <c r="M24" s="167"/>
+      <c r="N24" s="167"/>
+      <c r="O24" s="167"/>
+      <c r="P24" s="167"/>
+      <c r="Q24" s="167"/>
+      <c r="R24" s="167"/>
       <c r="S24" s="10"/>
     </row>
     <row r="25" ht="13.65" customHeight="1">
-      <c r="A25" t="s" s="153">
+      <c r="A25" t="s" s="170">
         <v>24</v>
       </c>
-      <c r="B25" s="149"/>
-      <c r="C25" s="150"/>
-      <c r="D25" s="150"/>
-      <c r="E25" s="150"/>
-      <c r="F25" s="150"/>
-      <c r="G25" s="150"/>
-      <c r="H25" s="150"/>
-      <c r="I25" s="150"/>
-      <c r="J25" s="150"/>
-      <c r="K25" s="150"/>
-      <c r="L25" s="150"/>
-      <c r="M25" s="150"/>
-      <c r="N25" s="150"/>
-      <c r="O25" s="150"/>
-      <c r="P25" s="150"/>
-      <c r="Q25" s="150"/>
-      <c r="R25" s="150"/>
+      <c r="B25" s="166"/>
+      <c r="C25" s="167"/>
+      <c r="D25" s="167"/>
+      <c r="E25" s="167"/>
+      <c r="F25" s="167"/>
+      <c r="G25" s="167"/>
+      <c r="H25" s="167"/>
+      <c r="I25" s="167"/>
+      <c r="J25" s="167"/>
+      <c r="K25" s="167"/>
+      <c r="L25" s="167"/>
+      <c r="M25" s="167"/>
+      <c r="N25" s="167"/>
+      <c r="O25" s="167"/>
+      <c r="P25" s="167"/>
+      <c r="Q25" s="167"/>
+      <c r="R25" s="167"/>
       <c r="S25" s="10"/>
     </row>
     <row r="26" ht="13.65" customHeight="1">
-      <c r="A26" t="s" s="154">
+      <c r="A26" t="s" s="171">
         <v>25</v>
       </c>
-      <c r="B26" s="149"/>
-      <c r="C26" s="150"/>
-      <c r="D26" s="150"/>
-      <c r="E26" s="150"/>
-      <c r="F26" s="150"/>
-      <c r="G26" s="150"/>
-      <c r="H26" s="150"/>
-      <c r="I26" s="150"/>
-      <c r="J26" s="150"/>
-      <c r="K26" s="150"/>
-      <c r="L26" s="150"/>
-      <c r="M26" s="150"/>
-      <c r="N26" s="150"/>
-      <c r="O26" s="150"/>
-      <c r="P26" s="150"/>
-      <c r="Q26" s="150"/>
-      <c r="R26" s="150"/>
+      <c r="B26" s="166"/>
+      <c r="C26" s="167"/>
+      <c r="D26" s="167"/>
+      <c r="E26" s="167"/>
+      <c r="F26" s="167"/>
+      <c r="G26" s="167"/>
+      <c r="H26" s="167"/>
+      <c r="I26" s="167"/>
+      <c r="J26" s="167"/>
+      <c r="K26" s="167"/>
+      <c r="L26" s="167"/>
+      <c r="M26" s="167"/>
+      <c r="N26" s="167"/>
+      <c r="O26" s="167"/>
+      <c r="P26" s="167"/>
+      <c r="Q26" s="167"/>
+      <c r="R26" s="167"/>
       <c r="S26" s="10"/>
     </row>
     <row r="27" ht="13.65" customHeight="1">
-      <c r="A27" t="s" s="155">
+      <c r="A27" t="s" s="172">
         <v>26</v>
       </c>
-      <c r="B27" s="149"/>
-      <c r="C27" s="150"/>
-      <c r="D27" s="150"/>
-      <c r="E27" s="150"/>
-      <c r="F27" s="150"/>
-      <c r="G27" s="150"/>
-      <c r="H27" s="150"/>
-      <c r="I27" s="150"/>
-      <c r="J27" s="150"/>
-      <c r="K27" s="150"/>
-      <c r="L27" s="150"/>
-      <c r="M27" s="150"/>
-      <c r="N27" s="150"/>
-      <c r="O27" s="150"/>
-      <c r="P27" s="150"/>
-      <c r="Q27" s="150"/>
-      <c r="R27" s="150"/>
+      <c r="B27" s="166"/>
+      <c r="C27" s="167"/>
+      <c r="D27" s="167"/>
+      <c r="E27" s="167"/>
+      <c r="F27" s="167"/>
+      <c r="G27" s="167"/>
+      <c r="H27" s="167"/>
+      <c r="I27" s="167"/>
+      <c r="J27" s="167"/>
+      <c r="K27" s="167"/>
+      <c r="L27" s="167"/>
+      <c r="M27" s="167"/>
+      <c r="N27" s="167"/>
+      <c r="O27" s="167"/>
+      <c r="P27" s="167"/>
+      <c r="Q27" s="167"/>
+      <c r="R27" s="167"/>
       <c r="S27" s="10"/>
     </row>
     <row r="28" ht="13.65" customHeight="1">
-      <c r="A28" t="s" s="156">
+      <c r="A28" t="s" s="173">
         <v>27</v>
       </c>
-      <c r="B28" s="149"/>
-      <c r="C28" s="150"/>
-      <c r="D28" s="150"/>
-      <c r="E28" s="150"/>
-      <c r="F28" s="150"/>
-      <c r="G28" s="150"/>
-      <c r="H28" s="150"/>
-      <c r="I28" s="150"/>
-      <c r="J28" s="150"/>
-      <c r="K28" s="150"/>
-      <c r="L28" s="150"/>
-      <c r="M28" s="150"/>
-      <c r="N28" s="150"/>
-      <c r="O28" s="150"/>
-      <c r="P28" s="150"/>
-      <c r="Q28" s="150"/>
-      <c r="R28" s="150"/>
+      <c r="B28" s="166"/>
+      <c r="C28" s="167"/>
+      <c r="D28" s="167"/>
+      <c r="E28" s="167"/>
+      <c r="F28" s="167"/>
+      <c r="G28" s="167"/>
+      <c r="H28" s="167"/>
+      <c r="I28" s="167"/>
+      <c r="J28" s="167"/>
+      <c r="K28" s="167"/>
+      <c r="L28" s="167"/>
+      <c r="M28" s="167"/>
+      <c r="N28" s="167"/>
+      <c r="O28" s="167"/>
+      <c r="P28" s="167"/>
+      <c r="Q28" s="167"/>
+      <c r="R28" s="167"/>
       <c r="S28" s="10"/>
     </row>
     <row r="29" ht="13.65" customHeight="1">
-      <c r="A29" t="s" s="157">
+      <c r="A29" t="s" s="174">
         <v>28</v>
       </c>
-      <c r="B29" s="149"/>
-      <c r="C29" s="150"/>
-      <c r="D29" s="150"/>
-      <c r="E29" s="150"/>
-      <c r="F29" s="150"/>
-      <c r="G29" s="150"/>
-      <c r="H29" s="150"/>
-      <c r="I29" s="150"/>
-      <c r="J29" s="150"/>
-      <c r="K29" s="150"/>
-      <c r="L29" s="150"/>
-      <c r="M29" s="150"/>
-      <c r="N29" s="150"/>
-      <c r="O29" s="150"/>
-      <c r="P29" s="150"/>
-      <c r="Q29" s="150"/>
-      <c r="R29" s="150"/>
+      <c r="B29" s="166"/>
+      <c r="C29" s="167"/>
+      <c r="D29" s="167"/>
+      <c r="E29" s="167"/>
+      <c r="F29" s="167"/>
+      <c r="G29" s="167"/>
+      <c r="H29" s="167"/>
+      <c r="I29" s="167"/>
+      <c r="J29" s="167"/>
+      <c r="K29" s="167"/>
+      <c r="L29" s="167"/>
+      <c r="M29" s="167"/>
+      <c r="N29" s="167"/>
+      <c r="O29" s="167"/>
+      <c r="P29" s="167"/>
+      <c r="Q29" s="167"/>
+      <c r="R29" s="167"/>
       <c r="S29" s="10"/>
     </row>
     <row r="30" ht="13.65" customHeight="1">
-      <c r="A30" t="s" s="158">
+      <c r="A30" t="s" s="175">
         <v>29</v>
       </c>
-      <c r="B30" t="s" s="159">
+      <c r="B30" t="s" s="176">
         <v>2</v>
       </c>
-      <c r="C30" s="150"/>
-      <c r="D30" s="150"/>
-      <c r="E30" s="150"/>
-      <c r="F30" s="150"/>
-      <c r="G30" s="150"/>
-      <c r="H30" s="150"/>
-      <c r="I30" s="150"/>
-      <c r="J30" s="150"/>
-      <c r="K30" s="150"/>
-      <c r="L30" s="150"/>
-      <c r="M30" s="150"/>
-      <c r="N30" s="150"/>
-      <c r="O30" s="150"/>
-      <c r="P30" s="150"/>
-      <c r="Q30" s="150"/>
-      <c r="R30" s="150"/>
+      <c r="C30" s="167"/>
+      <c r="D30" s="167"/>
+      <c r="E30" s="167"/>
+      <c r="F30" s="167"/>
+      <c r="G30" s="167"/>
+      <c r="H30" s="167"/>
+      <c r="I30" s="167"/>
+      <c r="J30" s="167"/>
+      <c r="K30" s="167"/>
+      <c r="L30" s="167"/>
+      <c r="M30" s="167"/>
+      <c r="N30" s="167"/>
+      <c r="O30" s="167"/>
+      <c r="P30" s="167"/>
+      <c r="Q30" s="167"/>
+      <c r="R30" s="167"/>
       <c r="S30" s="10"/>
     </row>
     <row r="31" ht="13.65" customHeight="1">
-      <c r="A31" t="s" s="160">
+      <c r="A31" t="s" s="177">
         <v>30</v>
       </c>
-      <c r="B31" t="s" s="159">
+      <c r="B31" t="s" s="176">
         <v>10</v>
       </c>
-      <c r="C31" t="s" s="159">
+      <c r="C31" t="s" s="176">
         <v>10</v>
       </c>
-      <c r="D31" s="150"/>
-      <c r="E31" s="150"/>
-      <c r="F31" s="150"/>
-      <c r="G31" s="150"/>
-      <c r="H31" s="150"/>
-      <c r="I31" s="150"/>
-      <c r="J31" s="150"/>
-      <c r="K31" s="150"/>
-      <c r="L31" s="150"/>
-      <c r="M31" s="150"/>
-      <c r="N31" s="150"/>
-      <c r="O31" s="150"/>
-      <c r="P31" s="150"/>
-      <c r="Q31" s="150"/>
-      <c r="R31" s="150"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="167"/>
+      <c r="G31" s="167"/>
+      <c r="H31" s="167"/>
+      <c r="I31" s="167"/>
+      <c r="J31" s="167"/>
+      <c r="K31" s="167"/>
+      <c r="L31" s="167"/>
+      <c r="M31" s="167"/>
+      <c r="N31" s="167"/>
+      <c r="O31" s="167"/>
+      <c r="P31" s="167"/>
+      <c r="Q31" s="167"/>
+      <c r="R31" s="167"/>
       <c r="S31" s="10"/>
     </row>
     <row r="32" ht="13.65" customHeight="1">
       <c r="A32" s="10"/>
-      <c r="B32" s="150"/>
-      <c r="C32" s="150"/>
-      <c r="D32" s="150"/>
-      <c r="E32" s="150"/>
-      <c r="F32" s="150"/>
-      <c r="G32" s="150"/>
-      <c r="H32" s="150"/>
-      <c r="I32" s="150"/>
-      <c r="J32" s="150"/>
-      <c r="K32" s="150"/>
-      <c r="L32" s="150"/>
-      <c r="M32" s="150"/>
-      <c r="N32" s="150"/>
-      <c r="O32" s="150"/>
-      <c r="P32" s="150"/>
-      <c r="Q32" s="150"/>
-      <c r="R32" s="150"/>
+      <c r="B32" s="167"/>
+      <c r="C32" s="167"/>
+      <c r="D32" s="167"/>
+      <c r="E32" s="167"/>
+      <c r="F32" s="167"/>
+      <c r="G32" s="167"/>
+      <c r="H32" s="167"/>
+      <c r="I32" s="167"/>
+      <c r="J32" s="167"/>
+      <c r="K32" s="167"/>
+      <c r="L32" s="167"/>
+      <c r="M32" s="167"/>
+      <c r="N32" s="167"/>
+      <c r="O32" s="167"/>
+      <c r="P32" s="167"/>
+      <c r="Q32" s="167"/>
+      <c r="R32" s="167"/>
       <c r="S32" s="10"/>
     </row>
     <row r="33" ht="13.65" customHeight="1">
-      <c r="A33" t="s" s="161">
+      <c r="A33" t="s" s="178">
         <v>31</v>
       </c>
-      <c r="B33" t="s" s="162">
+      <c r="B33" t="s" s="179">
         <v>32</v>
       </c>
-      <c r="C33" s="163"/>
-      <c r="D33" s="150"/>
-      <c r="E33" s="150"/>
-      <c r="F33" s="150"/>
-      <c r="G33" s="150"/>
-      <c r="H33" s="150"/>
-      <c r="I33" s="150"/>
-      <c r="J33" s="150"/>
-      <c r="K33" s="150"/>
-      <c r="L33" s="150"/>
-      <c r="M33" s="150"/>
-      <c r="N33" s="150"/>
-      <c r="O33" s="150"/>
-      <c r="P33" s="150"/>
-      <c r="Q33" s="150"/>
-      <c r="R33" s="150"/>
+      <c r="C33" s="180"/>
+      <c r="D33" s="167"/>
+      <c r="E33" s="167"/>
+      <c r="F33" s="167"/>
+      <c r="G33" s="167"/>
+      <c r="H33" s="167"/>
+      <c r="I33" s="167"/>
+      <c r="J33" s="167"/>
+      <c r="K33" s="167"/>
+      <c r="L33" s="167"/>
+      <c r="M33" s="167"/>
+      <c r="N33" s="167"/>
+      <c r="O33" s="167"/>
+      <c r="P33" s="167"/>
+      <c r="Q33" s="167"/>
+      <c r="R33" s="167"/>
       <c r="S33" s="10"/>
     </row>
     <row r="34" ht="13.65" customHeight="1">
-      <c r="A34" t="s" s="160">
+      <c r="A34" t="s" s="177">
         <v>33</v>
       </c>
-      <c r="B34" s="164"/>
-      <c r="C34" s="164"/>
-      <c r="D34" s="164"/>
-      <c r="E34" s="164"/>
-      <c r="F34" s="164"/>
-      <c r="G34" s="164"/>
-      <c r="H34" s="164"/>
-      <c r="I34" s="164"/>
-      <c r="J34" s="164"/>
-      <c r="K34" s="164"/>
-      <c r="L34" s="164"/>
-      <c r="M34" s="150"/>
-      <c r="N34" s="150"/>
-      <c r="O34" s="150"/>
-      <c r="P34" s="150"/>
-      <c r="Q34" s="150"/>
-      <c r="R34" s="150"/>
+      <c r="B34" s="181"/>
+      <c r="C34" s="181"/>
+      <c r="D34" s="181"/>
+      <c r="E34" s="181"/>
+      <c r="F34" s="181"/>
+      <c r="G34" s="181"/>
+      <c r="H34" s="181"/>
+      <c r="I34" s="181"/>
+      <c r="J34" s="181"/>
+      <c r="K34" s="181"/>
+      <c r="L34" s="181"/>
+      <c r="M34" s="167"/>
+      <c r="N34" s="167"/>
+      <c r="O34" s="167"/>
+      <c r="P34" s="167"/>
+      <c r="Q34" s="167"/>
+      <c r="R34" s="167"/>
       <c r="S34" s="10"/>
     </row>
     <row r="35" ht="13.65" customHeight="1">
-      <c r="A35" t="s" s="165">
+      <c r="A35" t="s" s="182">
         <v>34</v>
       </c>
-      <c r="B35" s="166">
+      <c r="B35" s="183">
         <v>0</v>
       </c>
-      <c r="C35" s="167">
+      <c r="C35" s="184">
         <v>1</v>
       </c>
-      <c r="D35" s="166">
+      <c r="D35" s="183">
         <v>2</v>
       </c>
-      <c r="E35" s="168">
+      <c r="E35" s="185">
         <v>3</v>
       </c>
-      <c r="F35" s="169">
+      <c r="F35" s="186">
         <v>4</v>
       </c>
-      <c r="G35" s="170">
+      <c r="G35" s="187">
         <v>5</v>
       </c>
-      <c r="H35" s="168">
+      <c r="H35" s="185">
         <v>6</v>
       </c>
-      <c r="I35" s="167">
+      <c r="I35" s="184">
         <v>7</v>
       </c>
-      <c r="J35" s="166">
+      <c r="J35" s="183">
         <v>8</v>
       </c>
-      <c r="K35" s="168">
+      <c r="K35" s="185">
         <v>9</v>
       </c>
-      <c r="L35" s="167">
+      <c r="L35" s="184">
         <v>10</v>
       </c>
-      <c r="M35" s="149"/>
-      <c r="N35" s="150"/>
-      <c r="O35" s="150"/>
-      <c r="P35" s="150"/>
-      <c r="Q35" s="150"/>
-      <c r="R35" s="150"/>
+      <c r="M35" s="166"/>
+      <c r="N35" s="167"/>
+      <c r="O35" s="167"/>
+      <c r="P35" s="167"/>
+      <c r="Q35" s="167"/>
+      <c r="R35" s="167"/>
       <c r="S35" s="10"/>
     </row>
     <row r="36" ht="13.65" customHeight="1">
-      <c r="A36" t="s" s="165">
+      <c r="A36" t="s" s="182">
         <v>21</v>
       </c>
-      <c r="B36" t="s" s="171">
+      <c r="B36" t="s" s="188">
         <v>4</v>
       </c>
-      <c r="C36" t="s" s="171">
+      <c r="C36" t="s" s="188">
         <v>5</v>
       </c>
-      <c r="D36" t="s" s="171">
+      <c r="D36" t="s" s="188">
         <v>5</v>
       </c>
-      <c r="E36" t="s" s="171">
+      <c r="E36" t="s" s="188">
         <v>8</v>
       </c>
-      <c r="F36" s="172"/>
-      <c r="G36" s="173"/>
-      <c r="H36" s="173"/>
-      <c r="I36" s="173"/>
-      <c r="J36" s="173"/>
-      <c r="K36" s="173"/>
-      <c r="L36" s="173"/>
-      <c r="M36" s="150"/>
-      <c r="N36" s="150"/>
-      <c r="O36" s="150"/>
-      <c r="P36" s="150"/>
-      <c r="Q36" s="150"/>
-      <c r="R36" s="150"/>
+      <c r="F36" s="189"/>
+      <c r="G36" s="190"/>
+      <c r="H36" s="190"/>
+      <c r="I36" s="190"/>
+      <c r="J36" s="190"/>
+      <c r="K36" s="190"/>
+      <c r="L36" s="190"/>
+      <c r="M36" s="167"/>
+      <c r="N36" s="167"/>
+      <c r="O36" s="167"/>
+      <c r="P36" s="167"/>
+      <c r="Q36" s="167"/>
+      <c r="R36" s="167"/>
       <c r="S36" s="10"/>
     </row>
     <row r="37" ht="13.65" customHeight="1">
-      <c r="A37" t="s" s="165">
+      <c r="A37" t="s" s="182">
         <v>35</v>
       </c>
-      <c r="B37" t="s" s="174">
+      <c r="B37" t="s" s="191">
         <v>9</v>
       </c>
-      <c r="C37" t="s" s="174">
+      <c r="C37" t="s" s="191">
         <v>3</v>
       </c>
-      <c r="D37" t="s" s="174">
+      <c r="D37" t="s" s="191">
         <v>12</v>
       </c>
-      <c r="E37" s="172"/>
-      <c r="F37" s="150"/>
-      <c r="G37" s="150"/>
-      <c r="H37" s="150"/>
-      <c r="I37" s="150"/>
-      <c r="J37" s="150"/>
-      <c r="K37" s="150"/>
-      <c r="L37" s="150"/>
-      <c r="M37" s="150"/>
-      <c r="N37" s="150"/>
-      <c r="O37" s="150"/>
-      <c r="P37" s="150"/>
-      <c r="Q37" s="150"/>
-      <c r="R37" s="150"/>
+      <c r="E37" s="189"/>
+      <c r="F37" s="167"/>
+      <c r="G37" s="167"/>
+      <c r="H37" s="167"/>
+      <c r="I37" s="167"/>
+      <c r="J37" s="167"/>
+      <c r="K37" s="167"/>
+      <c r="L37" s="167"/>
+      <c r="M37" s="167"/>
+      <c r="N37" s="167"/>
+      <c r="O37" s="167"/>
+      <c r="P37" s="167"/>
+      <c r="Q37" s="167"/>
+      <c r="R37" s="167"/>
       <c r="S37" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="S4:S8"/>
-    <mergeCell ref="S14:S18"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="F21:N21"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="S4:S9"/>
+    <mergeCell ref="S13:S18"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>